<commit_message>
more updates to figures
</commit_message>
<xml_diff>
--- a/figures/target_describe.xlsx
+++ b/figures/target_describe.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Mean</t>
   </si>
@@ -32,21 +32,26 @@
   </si>
   <si>
     <t xml:space="preserve">Maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurtosis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -67,6 +72,7 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -120,7 +126,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -141,13 +151,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.51"/>
   </cols>
@@ -156,7 +166,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="2" t="n">
         <v>3395.380184</v>
       </c>
     </row>
@@ -164,7 +174,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>11626.950749</v>
       </c>
     </row>
@@ -172,31 +182,31 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>0.25</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>946</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>1400</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>0.75</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>2800</v>
       </c>
     </row>
@@ -204,8 +214,16 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>843300</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1832.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>